<commit_message>
updated before transfer to Office 365 21-05-2019
</commit_message>
<xml_diff>
--- a/VBA_Button_On_Excel.xlsx
+++ b/VBA_Button_On_Excel.xlsx
@@ -2,20 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yaoa\Alan_HD\Alan_Work\HD_IT\HD_VBA\VBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12045"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12045" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511" refMode="R1C1" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -144,6 +145,125 @@
         <a:xfrm>
           <a:off x="133350" y="2857500"/>
           <a:ext cx="13771428" cy="6647619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>255924</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>133054</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="276225" y="238125"/>
+          <a:ext cx="10009524" cy="2371429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>398857</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>76039</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="276225" y="2981325"/>
+          <a:ext cx="9542857" cy="1285714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>94552</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>113519</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="276225" y="4343400"/>
+          <a:ext cx="5580952" cy="6247619"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -418,9 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Z16" sqref="Z16"/>
     </sheetView>
   </sheetViews>
@@ -434,6 +555,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.140625" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.15748031496062992" right="0.35433070866141736" top="0.15748031496062992" bottom="0.25" header="0.15748031496062992" footer="0.15748031496062992"/>
+  <pageSetup paperSize="9" scale="70" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>